<commit_message>
bikin biar ga ada duplikat masuk di mhs
</commit_message>
<xml_diff>
--- a/FIX_Data Mahasiswa Dummy.xlsx
+++ b/FIX_Data Mahasiswa Dummy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zahira\Documents\1 STIS\STIS smt 5\1 Project RPL\STIS-GRAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248B9D07-8EC8-4203-9D02-A5D91ACFD5F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654F01FA-6768-4253-8A80-C6E403637584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{F4B6EACE-16C0-48E0-959E-92E10067F066}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F4B6EACE-16C0-48E0-959E-92E10067F066}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="202">
   <si>
     <t>NIM</t>
   </si>
@@ -659,6 +659,96 @@
   </si>
   <si>
     <t>Daerah Asal</t>
+  </si>
+  <si>
+    <t>Anisa Rachman</t>
+  </si>
+  <si>
+    <t>4EK6</t>
+  </si>
+  <si>
+    <t>0819XXXXXX55</t>
+  </si>
+  <si>
+    <t>Banda Aceh</t>
+  </si>
+  <si>
+    <t>Evaluasi Kinerja Keuangan Bank Konvensional Pasca Pandemi</t>
+  </si>
+  <si>
+    <t>Samsul Rachman</t>
+  </si>
+  <si>
+    <t>Dicky Satria</t>
+  </si>
+  <si>
+    <t>4ST7</t>
+  </si>
+  <si>
+    <t>0853XXXXXX66</t>
+  </si>
+  <si>
+    <t>Ambon</t>
+  </si>
+  <si>
+    <t>Optimasi Penjadwalan Tenaga Kerja Menggunakan Algoritma Genetika</t>
+  </si>
+  <si>
+    <t>Rita Satria</t>
+  </si>
+  <si>
+    <t>Lana Azhari</t>
+  </si>
+  <si>
+    <t>4KS8</t>
+  </si>
+  <si>
+    <t>0877XXXXXX77</t>
+  </si>
+  <si>
+    <t>Jambi</t>
+  </si>
+  <si>
+    <t>Sistem Rekomendasi Destinasi Wisata Berbasis Collaborative Filtering</t>
+  </si>
+  <si>
+    <t>Rudi Azhari</t>
+  </si>
+  <si>
+    <t>Gilang Pratama</t>
+  </si>
+  <si>
+    <t>4EK9</t>
+  </si>
+  <si>
+    <t>0856XXXXXX88</t>
+  </si>
+  <si>
+    <t>Padang</t>
+  </si>
+  <si>
+    <t>Analisis Perilaku Konsumen Terhadap Produk Ramah Lingkungan</t>
+  </si>
+  <si>
+    <t>Wati Pratama</t>
+  </si>
+  <si>
+    <t>Nurul Huda</t>
+  </si>
+  <si>
+    <t>4ST10</t>
+  </si>
+  <si>
+    <t>0812XXXXXX99</t>
+  </si>
+  <si>
+    <t>Palangkaraya</t>
+  </si>
+  <si>
+    <t>Analisis Faktor-Faktor yang Mempengaruhi Tingkat Kelulusan Tepat Waktu</t>
+  </si>
+  <si>
+    <t>Lukman Huda</t>
   </si>
 </sst>
 </file>
@@ -729,13 +819,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" readingOrder="1"/>
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" readingOrder="1"/>
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1051,24 +1142,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD9C136-DFB1-4DFF-9871-80B6B94F26E2}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="F3" zoomScale="71" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="69.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="77.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1104,806 +1196,967 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>2018001</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>2018002</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <v>2018003</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <v>2018004</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
+      <c r="A6" s="3">
         <v>2018005</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
+      <c r="A7" s="3">
         <v>2018006</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
+      <c r="A8" s="3">
         <v>2018007</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
+      <c r="A9" s="3">
         <v>2018008</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
+      <c r="A10" s="3">
         <v>2018009</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
+      <c r="A11" s="3">
         <v>2018010</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2">
+      <c r="A12" s="3">
         <v>2018011</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
+      <c r="A13" s="3">
         <v>2018012</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
+      <c r="A14" s="3">
         <v>2018013</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="3" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
+      <c r="A15" s="3">
         <v>2018014</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
+      <c r="A16" s="3">
         <v>2018015</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="3" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
+      <c r="A17" s="3">
         <v>2018016</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I17" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="3" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
+      <c r="A18" s="3">
         <v>2018017</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="3" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2">
+      <c r="A19" s="3">
         <v>2018018</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" s="3" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2">
+      <c r="A20" s="3">
         <v>2018019</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I20" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="J20" s="3" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2">
+      <c r="A21" s="3">
         <v>2018020</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="I21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J21" s="3" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2">
+      <c r="A22" s="3">
         <v>2018021</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="I22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="J22" s="3" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2">
+      <c r="A23" s="3">
         <v>2018022</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="I23" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="J23" s="3" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2">
+      <c r="A24" s="3">
         <v>2018023</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H24" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="I24" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="J24" s="3" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2">
+      <c r="A25" s="3">
         <v>2018024</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H25" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="I25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="J25" s="3" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="2">
+      <c r="A26" s="3">
         <v>2018025</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H26" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="I26" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="J26" s="3" t="s">
         <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="3">
+        <v>2018026</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="3">
+        <v>2018027</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="3">
+        <v>2018028</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="3">
+        <v>2018029</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="3">
+        <v>2018030</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>